<commit_message>
Hardware Libraries added and Calculation updated
</commit_message>
<xml_diff>
--- a/Hardware/Pro/Kalkulation.xlsx
+++ b/Hardware/Pro/Kalkulation.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37540" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21460" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
+    <sheet name="Blatt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="BOM" localSheetId="0">Stückliste!$A$2:$G$33</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="152">
   <si>
     <t>Qty</t>
   </si>
@@ -509,9 +510,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ &quot;€&quot;_-;\-* #,##0.0000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000\ &quot;€&quot;_-;\-* #,##0.0000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -557,8 +558,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,8 +584,20 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -610,8 +629,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -620,8 +695,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -635,13 +711,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="7" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8"/>
@@ -650,48 +748,6 @@
     <cellStyle name="Währung" xfId="6" builtinId="4"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -736,16 +792,58 @@
       <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ &quot;€&quot;_-;\-* #,##0.0000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ &quot;€&quot;_-;\-* #,##0.0000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0000\ &quot;€&quot;_-;\-* #,##0.0000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0000\ &quot;€&quot;_-;\-* #,##0.0000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -764,38 +862,38 @@
   <autoFilter ref="A2:P33"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Qty" totalsRowLabel="Ergebnis"/>
-    <tableColumn id="9" name="Farnell" dataDxfId="15" totalsRowDxfId="6"/>
+    <tableColumn id="9" name="Farnell" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="2" name="Value"/>
     <tableColumn id="3" name="Device"/>
     <tableColumn id="4" name="Package"/>
     <tableColumn id="5" name="Parts"/>
     <tableColumn id="6" name="Description"/>
-    <tableColumn id="10" name="Menge" dataDxfId="14">
+    <tableColumn id="10" name="Menge" dataDxfId="13">
       <calculatedColumnFormula>$I$1*Tabelle2[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Einzelpreis" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="5" dataCellStyle="Währung">
+    <tableColumn id="11" name="Einzelpreis" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Währung">
       <totalsRowFormula>Tabelle2[[#Totals],[Positionspreis]]/I1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" name="Positionspreis" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="4" dataCellStyle="Währung">
+    <tableColumn id="12" name="Positionspreis" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Währung">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Menge]]*Tabelle2[[#This Row],[Einzelpreis]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="ohne BLE" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="3" dataCellStyle="Währung">
+    <tableColumn id="19" name="ohne BLE" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Währung">
       <totalsRowFormula>SUBTOTAL(109,Tabelle2[ohne BLE]) / I1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" name="Menge2" dataDxfId="11">
+    <tableColumn id="13" name="Menge2" dataDxfId="6">
       <calculatedColumnFormula>$M$1*Tabelle2[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Einzelpreis2" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="2" dataCellStyle="Währung">
+    <tableColumn id="14" name="Einzelpreis2" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Währung">
       <totalsRowFormula>Tabelle2[[#Totals],[Positionspreis2]]/M1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" name="Positionspreis2" totalsRowFunction="sum" totalsRowDxfId="1" dataCellStyle="Währung">
+    <tableColumn id="15" name="Positionspreis2" totalsRowFunction="sum" totalsRowDxfId="3" dataCellStyle="Währung">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Menge2]]*Tabelle2[[#This Row],[Einzelpreis2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="ohne BLE2" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="0" dataCellStyle="Währung">
+    <tableColumn id="17" name="ohne BLE2" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Währung">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Positionspreis2]]</calculatedColumnFormula>
       <totalsRowFormula>SUBTOTAL(109,Tabelle2[ohne BLE2])/M1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" name="Link" totalsRowFunction="custom" dataDxfId="9" dataCellStyle="Link">
+    <tableColumn id="18" name="Link" totalsRowFunction="custom" dataDxfId="0" dataCellStyle="Link">
       <calculatedColumnFormula>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle2[[#This Row],[Farnell]]), "Details")</calculatedColumnFormula>
       <totalsRowFormula>Tabelle2[[#Totals],[ohne BLE2]]/I1</totalsRowFormula>
     </tableColumn>
@@ -1128,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2939,7 +3037,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2949,4 +3046,550 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="80.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="10">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="35" customHeight="1">
+      <c r="A4" s="12">
+        <v>12</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="14">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="12">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="14">
+        <v>2</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="14">
+        <v>2</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="12">
+        <v>2</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="14">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="14">
+        <v>2</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="12">
+        <v>1</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="14">
+        <v>2</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="12">
+        <v>3</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="13">
+        <v>820</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="14">
+        <v>1</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="12">
+        <v>1</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="14">
+        <v>1</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="12">
+        <v>1</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="14">
+        <v>2</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="12">
+        <v>1</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="14">
+        <v>1</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="12">
+        <v>1</v>
+      </c>
+      <c r="B24" s="13">
+        <v>1734973</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="14">
+        <v>1</v>
+      </c>
+      <c r="B25" s="15">
+        <v>2443092</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="12">
+        <v>3</v>
+      </c>
+      <c r="B26" s="13">
+        <v>1830923</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="14">
+        <v>1</v>
+      </c>
+      <c r="B27" s="15">
+        <v>1103107</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="12">
+        <v>1</v>
+      </c>
+      <c r="B28" s="13">
+        <v>2466939</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="14">
+        <v>1</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="12">
+        <v>1</v>
+      </c>
+      <c r="B30" s="13">
+        <v>1830925</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="14">
+        <v>1</v>
+      </c>
+      <c r="B31" s="15">
+        <v>1645325</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Farnell OC's updated and paste pad reduction removed.
</commit_message>
<xml_diff>
--- a/Hardware/Pro/Kalkulation.xlsx
+++ b/Hardware/Pro/Kalkulation.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21460" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37620" windowHeight="23560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
-    <sheet name="Blatt1" sheetId="2" r:id="rId2"/>
+    <sheet name="Stückliste Proto" sheetId="1" r:id="rId1"/>
+    <sheet name="Stückliste Proto2" sheetId="3" r:id="rId2"/>
+    <sheet name="Blatt1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM" localSheetId="0">Stückliste!$A$2:$G$33</definedName>
+    <definedName name="BOM" localSheetId="0">'Stückliste Proto'!$A$2:$G$33</definedName>
+    <definedName name="BOM" localSheetId="1">'Stückliste Proto2'!$A$2:$I$27</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -42,11 +44,29 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="BOM.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:cem:xeniC:AnySense:Hardware:Pro:BOM.csv" decimal="," thousands="." semicolon="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="185">
   <si>
     <t>Qty</t>
   </si>
@@ -502,6 +522,105 @@
   </si>
   <si>
     <t>ohne BLE2</t>
+  </si>
+  <si>
+    <t>1.5K</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>C8, C12, C14, C15, C16, C30, C31</t>
+  </si>
+  <si>
+    <t>R3, R5, R9, R10, R12</t>
+  </si>
+  <si>
+    <t>15K</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2320776RL </t>
+  </si>
+  <si>
+    <t>C-EUC0603K</t>
+  </si>
+  <si>
+    <t>C0603K</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>1759409RL</t>
+  </si>
+  <si>
+    <t>22R</t>
+  </si>
+  <si>
+    <t>R1, R11</t>
+  </si>
+  <si>
+    <t>2320818RL</t>
+  </si>
+  <si>
+    <t>OSD, SENSOR, TELEM</t>
+  </si>
+  <si>
+    <t>Ab</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>LED Green</t>
+  </si>
+  <si>
+    <t>LED Red</t>
+  </si>
+  <si>
+    <t>LED Orange</t>
+  </si>
+  <si>
+    <t>Keramikvielschichtkondensator, SMD, Baureihe MC, 4.7 µF, ± 10%, X5R, 10 V</t>
+  </si>
+  <si>
+    <t>Keramikvielschichtkondensator, SMD, Baureihe MC, 1 µF, ± 10%, X5R, 25 V</t>
+  </si>
+  <si>
+    <t>Keramikvielschichtkondensator, SMD, Baureihe MC, 1 µF, ± 10%, X5R, 10 V</t>
+  </si>
+  <si>
+    <t>2302656RL</t>
+  </si>
+  <si>
+    <t>Dickschichtwiderstand, Oberflächenmont., Baureihe AEC-Q200 ERJ, 1.5 kohm, 100 mW, ± 1%, 50 V</t>
+  </si>
+  <si>
+    <t>Dickschichtwiderstand, Oberflächenmont., Baureihe AEC-Q200 ERJ, 15 kohm, 100 mW, ± 1%, 50 V</t>
+  </si>
+  <si>
+    <t>2302754RL</t>
+  </si>
+  <si>
+    <t>2302453RL</t>
+  </si>
+  <si>
+    <t>Dickschichtwiderstand, Oberflächenmont., Baureihe AEC-Q200 ERJ, 22 ohm, 100 mW, ± 1%, 50 V</t>
+  </si>
+  <si>
+    <t>820R</t>
   </si>
 </sst>
 </file>
@@ -686,7 +805,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -696,8 +815,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -735,11 +858,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8"/>
@@ -747,7 +875,19 @@
     <cellStyle name="Überschrift 1" xfId="7" builtinId="16"/>
     <cellStyle name="Währung" xfId="6" builtinId="4"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0000\ &quot;€&quot;_-;\-* #,##0.0000\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -857,45 +997,75 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="BOM" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="BOM" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:P34" totalsRowCount="1">
   <autoFilter ref="A2:P33"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Qty" totalsRowLabel="Ergebnis"/>
-    <tableColumn id="9" name="Farnell" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="9" name="Farnell" dataDxfId="19" totalsRowDxfId="18"/>
     <tableColumn id="2" name="Value"/>
     <tableColumn id="3" name="Device"/>
     <tableColumn id="4" name="Package"/>
     <tableColumn id="5" name="Parts"/>
     <tableColumn id="6" name="Description"/>
-    <tableColumn id="10" name="Menge" dataDxfId="13">
+    <tableColumn id="10" name="Menge" dataDxfId="17">
       <calculatedColumnFormula>$I$1*Tabelle2[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Einzelpreis" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Währung">
+    <tableColumn id="11" name="Einzelpreis" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Währung">
       <totalsRowFormula>Tabelle2[[#Totals],[Positionspreis]]/I1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" name="Positionspreis" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Währung">
+    <tableColumn id="12" name="Positionspreis" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Währung">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Menge]]*Tabelle2[[#This Row],[Einzelpreis]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="ohne BLE" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Währung">
+    <tableColumn id="19" name="ohne BLE" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Währung">
       <totalsRowFormula>SUBTOTAL(109,Tabelle2[ohne BLE]) / I1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" name="Menge2" dataDxfId="6">
+    <tableColumn id="13" name="Menge2" dataDxfId="10">
       <calculatedColumnFormula>$M$1*Tabelle2[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Einzelpreis2" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Währung">
+    <tableColumn id="14" name="Einzelpreis2" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Währung">
       <totalsRowFormula>Tabelle2[[#Totals],[Positionspreis2]]/M1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" name="Positionspreis2" totalsRowFunction="sum" totalsRowDxfId="3" dataCellStyle="Währung">
+    <tableColumn id="15" name="Positionspreis2" totalsRowFunction="sum" totalsRowDxfId="7" dataCellStyle="Währung">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Menge2]]*Tabelle2[[#This Row],[Einzelpreis2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="ohne BLE2" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Währung">
+    <tableColumn id="17" name="ohne BLE2" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Währung">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Positionspreis2]]</calculatedColumnFormula>
       <totalsRowFormula>SUBTOTAL(109,Tabelle2[ohne BLE2])/M1</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" name="Link" totalsRowFunction="custom" dataDxfId="0" dataCellStyle="Link">
+    <tableColumn id="18" name="Link" totalsRowFunction="custom" dataDxfId="4" dataCellStyle="Link">
       <calculatedColumnFormula>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle2[[#This Row],[Farnell]]), "Details")</calculatedColumnFormula>
       <totalsRowFormula>Tabelle2[[#Totals],[ohne BLE2]]/I1</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:K28" totalsRowCount="1">
+  <autoFilter ref="A2:K27"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Qty"/>
+    <tableColumn id="2" name="Farnell"/>
+    <tableColumn id="3" name="Value"/>
+    <tableColumn id="4" name="Device"/>
+    <tableColumn id="5" name="Package"/>
+    <tableColumn id="6" name="Parts"/>
+    <tableColumn id="7" name="Description"/>
+    <tableColumn id="11" name="Link" dataDxfId="3">
+      <calculatedColumnFormula>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Anzahl" dataDxfId="2">
+      <calculatedColumnFormula>$J$1*Tabelle1[[#This Row],[Qty]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="EP" dataDxfId="1" dataCellStyle="Währung"/>
+    <tableColumn id="10" name="Summe" totalsRowFunction="sum" dataDxfId="0">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1226,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1235,10 +1405,10 @@
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="80.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.5" customWidth="1"/>
     <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
@@ -3049,6 +3219,1029 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="I1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I3">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J3" s="7">
+        <v>6.3399999999999998E-2</v>
+      </c>
+      <c r="K3">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I4">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J4" s="7">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="K4">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I5">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J5" s="7">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="K5">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I6">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J6" s="7">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K6">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>3.4499999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I7">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>3500</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2E-3</v>
+      </c>
+      <c r="K7">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I8">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>2500</v>
+      </c>
+      <c r="J8" s="7">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="K8">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>14.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I9">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>1000</v>
+      </c>
+      <c r="J9" s="7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K9">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I10">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J10" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K10">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I11">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>1000</v>
+      </c>
+      <c r="J11" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K11">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I12">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J12" s="7">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K12">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>3.4499999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H13" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I13">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J13" s="7">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K13">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" t="s">
+        <v>176</v>
+      </c>
+      <c r="H14" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I14">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J14" s="7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K14">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" t="s">
+        <v>183</v>
+      </c>
+      <c r="H15" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I15">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>1000</v>
+      </c>
+      <c r="J15" s="7">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K15">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>6.8999999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" t="s">
+        <v>161</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>175</v>
+      </c>
+      <c r="H16" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I16">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>1000</v>
+      </c>
+      <c r="J16" s="7">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="K16">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>136</v>
+      </c>
+      <c r="H17" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I17">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>1500</v>
+      </c>
+      <c r="J17" s="7">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K17">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>10.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H18" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I18">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J18" s="7">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="K18">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" t="s">
+        <v>141</v>
+      </c>
+      <c r="H19" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I19">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>1000</v>
+      </c>
+      <c r="J19" s="7">
+        <v>7.51E-2</v>
+      </c>
+      <c r="K19">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>75.099999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H20" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I20">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J20" s="7">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="K20">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>242.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>1734973</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I21">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J21" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="K21">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2443092</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I22">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="K22">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>1830923</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I23">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>1500</v>
+      </c>
+      <c r="J23" s="7">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="K23">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1103107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I24">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="K24">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>2466939</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" t="s">
+        <v>148</v>
+      </c>
+      <c r="H25" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I25">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J25" s="7">
+        <v>4.87</v>
+      </c>
+      <c r="K25">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1830925</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I26">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="K26">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1645325</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE("http://de.farnell.com/a/b/c/dp/",Tabelle1[[#This Row],[Farnell]]), "Details")</f>
+        <v>Details</v>
+      </c>
+      <c r="I27">
+        <f>$J$1*Tabelle1[[#This Row],[Qty]]</f>
+        <v>500</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="K27">
+        <f>Tabelle1[[#This Row],[Anzahl]]*Tabelle1[[#This Row],[EP]]</f>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="K28">
+        <f>SUBTOTAL(109,Tabelle1[Summe])</f>
+        <v>5159.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>

</xml_diff>